<commit_message>
add dataset、split code and copyright cells
</commit_message>
<xml_diff>
--- a/transfer_learning_effect/data.xlsx
+++ b/transfer_learning_effect/data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\paper data\迁移学习效果\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\IEEE-paper\transfer_learning_effect\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{871DD7BD-BDB8-4CB8-89F0-71DFDB6F1DE2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F86747F-A925-46B7-89F8-5C8F145AE743}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,18 +21,6 @@
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="微软雅黑"/>
-        <family val="2"/>
-        <charset val="134"/>
-      </rPr>
-      <t>数据集大小</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
   <si>
     <r>
       <rPr>
@@ -79,6 +67,10 @@
       </rPr>
       <t>test_loss</t>
     </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dataset_size</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -139,15 +131,18 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -467,7 +462,7 @@
   <dimension ref="A1:AA201"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="A3:E10"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
@@ -505,20 +500,20 @@
       <c r="AA1" s="1"/>
     </row>
     <row r="2" spans="1:27" ht="15" x14ac:dyDescent="0.4">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>3</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>4</v>
       </c>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>

</xml_diff>